<commit_message>
environment.yml updated and modules wo a installer added to main notebook
</commit_message>
<xml_diff>
--- a/data/SD_AHBA_fdr0005_GTExbrainBG_GO_significant_genes.xlsx
+++ b/data/SD_AHBA_fdr0005_GTExbrainBG_GO_significant_genes.xlsx
@@ -4969,8 +4969,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009E9431FF1ED4534F8409F0DBD6EDFBB3" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f17474379f723092ba30ee0080e816cb">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d48fb685-4bd1-4676-b7e7-4e766cffcf89" xmlns:ns3="19e227d1-17ae-45de-a6d5-2758eb569cda" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d1b5788b327ea351b7cded7520d391" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E9431FF1ED4534F8409F0DBD6EDFBB3" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b76e4b1843cb2005c2068e501ab08d7">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d48fb685-4bd1-4676-b7e7-4e766cffcf89" xmlns:ns3="19e227d1-17ae-45de-a6d5-2758eb569cda" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2425b0773d2bcb9b3f2b4b9aa164747" ns2:_="" ns3:_="">
     <xsd:import namespace="d48fb685-4bd1-4676-b7e7-4e766cffcf89"/>
     <xsd:import namespace="19e227d1-17ae-45de-a6d5-2758eb569cda"/>
     <xsd:element name="properties">
@@ -5057,7 +5057,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="14ae72d6-1d51-44e0-a414-869ae22c088a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="14ae72d6-1d51-44e0-a414-869ae22c088a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -5068,7 +5068,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="19e227d1-17ae-45de-a6d5-2758eb569cda" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -5087,7 +5087,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -5115,8 +5115,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -5214,5 +5214,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D10C1495-342F-4C62-89E0-7947F1D42BEF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DC94A51-B149-420A-B0B1-2FD6876B5662}"/>
 </file>
</xml_diff>